<commit_message>
TAWA_SIQ document and TAWA_SystemRequirements have been modified
</commit_message>
<xml_diff>
--- a/TAWA_SIQ.xlsx
+++ b/TAWA_SIQ.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>From which source the top travel destinations appear statistics or ratings of the website?</t>
   </si>
@@ -77,6 +77,24 @@
   </si>
   <si>
     <t>TAWA_SIQ_008</t>
+  </si>
+  <si>
+    <t>User will choose the journey and book from the website, he/she can book going&amp;coming back or he/she can book going only.</t>
+  </si>
+  <si>
+    <t>By username and password.</t>
+  </si>
+  <si>
+    <t>Cash/Debit card.</t>
+  </si>
+  <si>
+    <t>Admin can add or delete users.</t>
+  </si>
+  <si>
+    <t>From users ratings.</t>
+  </si>
+  <si>
+    <t>Proposals</t>
   </si>
   <si>
     <r>
@@ -167,33 +185,56 @@
       <t xml:space="preserve">
 </t>
     </r>
-  </si>
-  <si>
-    <t>User will choose the journey and book from the website, he/she can book going&amp;coming back or he/she can book going only.</t>
-  </si>
-  <si>
-    <t>By username and password.</t>
-  </si>
-  <si>
-    <t>Cash/Debit card.</t>
-  </si>
-  <si>
-    <t>Admin can add or delete users.</t>
-  </si>
-  <si>
-    <t>From users ratings.</t>
-  </si>
-  <si>
-    <t>Performance(Throughput=1000,response time=5 seconds).</t>
-  </si>
-  <si>
-    <t>Proposals</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Author: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>esraa salah</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>TAWA_SIQ_009</t>
+  </si>
+  <si>
+    <t>What is the maximum length of the phone number field?</t>
+  </si>
+  <si>
+    <t>12 characters.</t>
   </si>
   <si>
     <t xml:space="preserve">For username contains Characters, numbers and Special characters only.
-For email and password contains Characters, numbers and Special characters and do not accept spaces.
+For email and password contains Characters, numbers and Special characters ,does not accept spaces and with length in betweeen 8 and 12 characters.
 For phone number field accepts numbers only.
-The required fields Username, email, password, fullname, phone. </t>
+The required fields Username, email, password, fullname, phone number. </t>
+  </si>
+  <si>
+    <t>Performance(Throughput=1000 request,response time=5 seconds).</t>
   </si>
 </sst>
 </file>
@@ -289,12 +330,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -317,6 +355,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -635,12 +677,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="100.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
+      <c r="A1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -655,122 +697,128 @@
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="6"/>
+    </row>
+    <row r="4" spans="1:16" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:16" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:16" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:16" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:16" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:16" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:16" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="1:16" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="7"/>
-    </row>
-    <row r="5" spans="1:16" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="7"/>
-    </row>
-    <row r="6" spans="1:16" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="7"/>
-    </row>
-    <row r="7" spans="1:16" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="7"/>
-    </row>
-    <row r="8" spans="1:16" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="7"/>
-    </row>
-    <row r="9" spans="1:16" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="8" t="s">
+      <c r="B11" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="7"/>
-    </row>
-    <row r="11" spans="1:16" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="1"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="11" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
comments were added to 'TAWA_ConfigurationManagementPlan_V1.0' document and 'TAWA_SIQ'document in the 'TAWA_PeerReviewSheet'document
</commit_message>
<xml_diff>
--- a/TAWA_SIQ.xlsx
+++ b/TAWA_SIQ.xlsx
@@ -294,7 +294,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -318,28 +318,70 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -352,13 +394,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,160 +715,149 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.109375" customWidth="1"/>
-    <col min="2" max="3" width="100.77734375" customWidth="1"/>
-    <col min="4" max="4" width="53.88671875" customWidth="1"/>
+    <col min="1" max="1" width="39.109375" style="13" customWidth="1"/>
+    <col min="2" max="3" width="100.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="53.88671875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="100.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" s="10" customFormat="1" ht="100.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-    </row>
-    <row r="2" spans="1:16" ht="21" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:4" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:16" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:16" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:16" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:16" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:16" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:16" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:4" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:16" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="11" t="s">
+      <c r="C11" s="7"/>
+      <c r="D11" s="4" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
The'TAWA_SIQ'document has been modified
</commit_message>
<xml_diff>
--- a/TAWA_SIQ.xlsx
+++ b/TAWA_SIQ.xlsx
@@ -88,9 +88,6 @@
     <t>Cash/Debit card.</t>
   </si>
   <si>
-    <t>Admin can add or delete users.</t>
-  </si>
-  <si>
     <t>From users ratings.</t>
   </si>
   <si>
@@ -235,6 +232,9 @@
   </si>
   <si>
     <t>Performance(Throughput=1000 request,response time=5 seconds).</t>
+  </si>
+  <si>
+    <t>Admin can add ,search and delete users.</t>
   </si>
 </sst>
 </file>
@@ -397,12 +397,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -411,6 +405,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -717,66 +717,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.109375" style="13" customWidth="1"/>
+    <col min="1" max="1" width="39.109375" style="11" customWidth="1"/>
     <col min="2" max="3" width="100.77734375" style="1" customWidth="1"/>
     <col min="4" max="4" width="53.88671875" style="1" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="10" customFormat="1" ht="100.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+    <row r="1" spans="1:4" s="8" customFormat="1" ht="100.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -788,7 +788,7 @@
       <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -800,19 +800,19 @@
       <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -824,21 +824,21 @@
       <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="100.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -850,15 +850,15 @@
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" ht="49.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Other questions have been added to 'TAWA_SIQ'document
</commit_message>
<xml_diff>
--- a/TAWA_SIQ.xlsx
+++ b/TAWA_SIQ.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>From which source the top travel destinations appear statistics or ratings of the website?</t>
   </si>
@@ -250,16 +250,23 @@
     <t>TAWA_SIQ_010</t>
   </si>
   <si>
-    <t>What are types of browsers within our scope?</t>
-  </si>
-  <si>
     <t>TAWA_SIQ_011</t>
   </si>
   <si>
     <t>How many flights can the user reserve?</t>
   </si>
   <si>
-    <t>Our proposal is : the user can reserve on flight at a specific time, but if the flights' dates do not overlap so the user can reserve any number of flights.</t>
+    <t>What are the types of browsers will be used in our scope?</t>
+  </si>
+  <si>
+    <t>The phone number field shouldn't exceed 20 characters in length</t>
+  </si>
+  <si>
+    <t>I believe our application should be supported on Chrome,FireFox, Edge,Safari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No, I am going to stick with the single flight per user and the user will be left with only  two options of booking: 
+Either to book a one-way ticket or to book a round-trip ticket. </t>
   </si>
 </sst>
 </file>
@@ -319,7 +326,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -343,51 +350,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -403,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -419,21 +387,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -742,28 +702,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.140625" style="11" customWidth="1"/>
-    <col min="2" max="3" width="100.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="53.85546875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="39.109375" style="8" customWidth="1"/>
+    <col min="2" max="3" width="100.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="53.88671875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="8" customFormat="1" ht="100.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:4" s="7" customFormat="1" ht="100.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-    </row>
-    <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+    </row>
+    <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -776,8 +736,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="100.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:4" ht="100.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -788,8 +748,8 @@
       </c>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" ht="100.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:4" ht="100.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -800,8 +760,8 @@
       </c>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" ht="100.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:4" ht="100.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -812,8 +772,8 @@
       </c>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" ht="100.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:4" ht="100.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -824,8 +784,8 @@
       </c>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" ht="100.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="1:4" ht="100.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -836,8 +796,8 @@
       </c>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" ht="100.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:4" ht="100.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -848,8 +808,8 @@
       </c>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:4" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -862,8 +822,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="100.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:4" ht="100.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -874,37 +834,43 @@
       </c>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:4" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="4" t="s">
+      <c r="C11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:4" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:4" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" spans="1:4" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="B13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="C13" s="5" t="s">
-        <v>37</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D13" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Other questions have been add to 'TAWA_SIQ'document
</commit_message>
<xml_diff>
--- a/TAWA_SIQ.xlsx
+++ b/TAWA_SIQ.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>From which source the top travel destinations appear statistics or ratings of the website?</t>
   </si>
@@ -250,16 +250,23 @@
     <t>TAWA_SIQ_010</t>
   </si>
   <si>
-    <t>What are types of browsers within our scope?</t>
-  </si>
-  <si>
     <t>TAWA_SIQ_011</t>
   </si>
   <si>
     <t>How many flights can the user reserve?</t>
   </si>
   <si>
-    <t>Our proposal is : the user can reserve on flight at a specific time, but if the flights' dates do not overlap so the user can reserve any number of flights.</t>
+    <t>What are the types of browsers will be used in our scope?</t>
+  </si>
+  <si>
+    <t>The phone number field shouldn't exceed 20 characters in length</t>
+  </si>
+  <si>
+    <t>I believe our application should be supported on Chrome,FireFox, Edge,Safari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No, I am going to stick with the single flight per user and the user will be left with only  two options of booking: 
+Either to book a one-way ticket or to book a round-trip ticket. </t>
   </si>
 </sst>
 </file>
@@ -319,7 +326,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -343,51 +350,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -403,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -419,21 +387,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -742,28 +702,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.140625" style="11" customWidth="1"/>
-    <col min="2" max="3" width="100.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="53.85546875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="39.109375" style="8" customWidth="1"/>
+    <col min="2" max="3" width="100.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="53.88671875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="8" customFormat="1" ht="100.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:4" s="7" customFormat="1" ht="100.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-    </row>
-    <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+    </row>
+    <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -776,8 +736,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="100.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:4" ht="100.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -788,8 +748,8 @@
       </c>
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:4" ht="100.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:4" ht="100.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -800,8 +760,8 @@
       </c>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" ht="100.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:4" ht="100.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -812,8 +772,8 @@
       </c>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" ht="100.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:4" ht="100.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -824,8 +784,8 @@
       </c>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" ht="100.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="1:4" ht="100.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -836,8 +796,8 @@
       </c>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" ht="100.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:4" ht="100.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -848,8 +808,8 @@
       </c>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:4" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -862,8 +822,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="100.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:4" ht="100.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -874,37 +834,43 @@
       </c>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:4" ht="49.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:4" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="4" t="s">
+      <c r="C11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:4" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:4" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" spans="1:4" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="B13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="C13" s="5" t="s">
-        <v>37</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D13" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Final updates to documents
</commit_message>
<xml_diff>
--- a/TAWA_SIQ.xlsx
+++ b/TAWA_SIQ.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>From which source the top travel destinations appear statistics or ratings of the website?</t>
   </si>
@@ -115,6 +115,52 @@
     <t>Admin can add ,search and delete users.</t>
   </si>
   <si>
+    <t>TAWA_SIQ_010</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_011</t>
+  </si>
+  <si>
+    <t>How many flights can the user reserve?</t>
+  </si>
+  <si>
+    <t>What are the types of browsers will be used in our scope?</t>
+  </si>
+  <si>
+    <t>The phone number field shouldn't exceed 20 characters in length</t>
+  </si>
+  <si>
+    <t>I believe our application should be supported on Chrome,FireFox, Edge,Safari</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No, I am going to stick with the single flight per user and the user will be left with only  two options of booking: 
+Either to book a one-way ticket or to book a round-trip ticket. </t>
+  </si>
+  <si>
+    <t>Revision Date</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Sara Sayed</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Adding three SIQs after replying from product owner .</t>
+  </si>
+  <si>
+    <t>Revised By</t>
+  </si>
+  <si>
+    <t>Version History</t>
+  </si>
+  <si>
+    <t>Update SIQs that contradict with SRS.</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">
 </t>
@@ -190,7 +236,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>27/4/2019</t>
+      <t>27/04/2019</t>
     </r>
     <r>
       <rPr>
@@ -232,7 +278,29 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>sraa Salah</t>
+      <t xml:space="preserve">sraa Salah
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Version</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:1.2</t>
     </r>
     <r>
       <rPr>
@@ -245,35 +313,13 @@
       <t xml:space="preserve">
 </t>
     </r>
-  </si>
-  <si>
-    <t>TAWA_SIQ_010</t>
-  </si>
-  <si>
-    <t>TAWA_SIQ_011</t>
-  </si>
-  <si>
-    <t>How many flights can the user reserve?</t>
-  </si>
-  <si>
-    <t>What are the types of browsers will be used in our scope?</t>
-  </si>
-  <si>
-    <t>The phone number field shouldn't exceed 20 characters in length</t>
-  </si>
-  <si>
-    <t>I believe our application should be supported on Chrome,FireFox, Edge,Safari</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No, I am going to stick with the single flight per user and the user will be left with only  two options of booking: 
-Either to book a one-way ticket or to book a round-trip ticket. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,6 +353,22 @@
       <b/>
       <sz val="16"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="2" tint="-0.89999084444715716"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -371,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -393,7 +455,26 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -700,181 +781,244 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.109375" style="8" customWidth="1"/>
-    <col min="2" max="3" width="100.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="53.88671875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="39.140625" style="8" customWidth="1"/>
+    <col min="2" max="3" width="100.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="53.85546875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="7" customFormat="1" ht="100.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:4" s="7" customFormat="1" ht="100.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+    </row>
+    <row r="2" spans="1:4" ht="100.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+    </row>
+    <row r="3" spans="1:4" s="12" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="14" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="16">
+        <v>43585</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="14" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="16">
+        <v>43587</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="14" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="16">
+        <v>43588</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="15">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="100.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" ht="100.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" ht="100.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" ht="100.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" ht="100.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" ht="100.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" ht="100.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="100.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" customFormat="1" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-    </row>
-    <row r="2" spans="1:4" ht="21" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="100.2" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" ht="100.2" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" ht="100.2" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" ht="100.2" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" ht="100.2" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" ht="100.2" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="100.2" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="B17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="D17" s="10"/>
+    </row>
+    <row r="18" spans="1:4" customFormat="1" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="B18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="10"/>
-    </row>
-    <row r="13" spans="1:4" customFormat="1" ht="70.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="5"/>
+      <c r="D18" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
New Questions had been added in TAWA_SIQ.xlsx document
</commit_message>
<xml_diff>
--- a/TAWA_SIQ.xlsx
+++ b/TAWA_SIQ.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
   <si>
     <t>From which source the top travel destinations appear statistics or ratings of the website?</t>
   </si>
@@ -313,6 +313,72 @@
       <t xml:space="preserve">
 </t>
     </r>
+  </si>
+  <si>
+    <t>TAWA_SIQ_012</t>
+  </si>
+  <si>
+    <t>What is the length of text fileds of  username , email and full name?</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_013</t>
+  </si>
+  <si>
+    <t>There is confirm password in sign up form?</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_014</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_015</t>
+  </si>
+  <si>
+    <t>according to the browser types, will we have compatibility in non-functional requirements?</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_016</t>
+  </si>
+  <si>
+    <t>the login page contain forget password link?</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_017</t>
+  </si>
+  <si>
+    <t>what is the type of error message in sign up and login forms?</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_018</t>
+  </si>
+  <si>
+    <t>the sign up is a link or button to redirect to the sign up form page?</t>
+  </si>
+  <si>
+    <t>the sign up in the sign up form is a link or button to submit the form?</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_019</t>
+  </si>
+  <si>
+    <t>the sign up in the login form is a link or button to submit the form?</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_020</t>
+  </si>
+  <si>
+    <t>there is login link in the sign up form?</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_021</t>
+  </si>
+  <si>
+    <t>there is sign up link in the login form?</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_022</t>
+  </si>
+  <si>
+    <t>the sign up and login in the navigation bar ?</t>
   </si>
 </sst>
 </file>
@@ -433,7 +499,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -470,6 +536,9 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -781,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,20 +865,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="7" customFormat="1" ht="100.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:4" ht="100.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="1:4" s="12" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
@@ -1014,6 +1083,94 @@
         <v>38</v>
       </c>
       <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
A repeated question has been deleted from'TAWA_SIQ'document
</commit_message>
<xml_diff>
--- a/TAWA_SIQ.xlsx
+++ b/TAWA_SIQ.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="id">Sheet1!$I$642941</definedName>
+    <definedName name="id">Sheet1!$I$642940</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="102">
   <si>
     <t>From which source the top travel destinations appear statistics or ratings of the website?</t>
   </si>
@@ -329,9 +329,6 @@
     <t>Is there a confirmation password field in the  sign up form?</t>
   </si>
   <si>
-    <t>The sign up field  is a link or button for the redirection to the sign up form page?</t>
-  </si>
-  <si>
     <t>According to the browser types, will we have compatibility in the non-functional requirements?</t>
   </si>
   <si>
@@ -402,9 +399,6 @@
   </si>
   <si>
     <t>TAWA_SIQ_039</t>
-  </si>
-  <si>
-    <t>TAWA_SIQ_040</t>
   </si>
   <si>
     <t>What is the scenario of the rating system?</t>
@@ -991,10 +985,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C33" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1288,7 +1282,7 @@
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F14" s="14">
         <v>43621</v>
@@ -1305,7 +1299,7 @@
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
       <c r="E15" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F15" s="14">
         <v>43621</v>
@@ -1322,7 +1316,7 @@
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F16" s="14">
         <v>43621</v>
@@ -1339,7 +1333,7 @@
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F17" s="14">
         <v>43621</v>
@@ -1356,7 +1350,7 @@
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F18" s="14">
         <v>43621</v>
@@ -1373,7 +1367,7 @@
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F19" s="14">
         <v>43621</v>
@@ -1385,12 +1379,12 @@
         <v>43</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F20" s="14">
         <v>43621</v>
@@ -1402,12 +1396,12 @@
         <v>44</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
       <c r="E21" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F21" s="14">
         <v>43621</v>
@@ -1419,12 +1413,12 @@
         <v>45</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F22" s="14">
         <v>43621</v>
@@ -1436,12 +1430,12 @@
         <v>46</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
       <c r="E23" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F23" s="14">
         <v>43621</v>
@@ -1453,12 +1447,12 @@
         <v>47</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F24" s="14">
         <v>43621</v>
@@ -1467,15 +1461,15 @@
     </row>
     <row r="25" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F25" s="14">
         <v>43621</v>
@@ -1484,15 +1478,15 @@
     </row>
     <row r="26" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
       <c r="E26" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F26" s="14">
         <v>43621</v>
@@ -1501,15 +1495,15 @@
     </row>
     <row r="27" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
       <c r="E27" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F27" s="14">
         <v>43621</v>
@@ -1518,15 +1512,15 @@
     </row>
     <row r="28" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
       <c r="E28" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F28" s="14">
         <v>43621</v>
@@ -1535,7 +1529,7 @@
     </row>
     <row r="29" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>88</v>
@@ -1543,7 +1537,7 @@
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
       <c r="E29" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F29" s="14">
         <v>43621</v>
@@ -1552,15 +1546,15 @@
     </row>
     <row r="30" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
       <c r="E30" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F30" s="14">
         <v>43621</v>
@@ -1569,15 +1563,15 @@
     </row>
     <row r="31" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
       <c r="E31" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F31" s="14">
         <v>43621</v>
@@ -1586,15 +1580,15 @@
     </row>
     <row r="32" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
       <c r="E32" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F32" s="14">
         <v>43621</v>
@@ -1603,15 +1597,15 @@
     </row>
     <row r="33" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
       <c r="E33" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F33" s="14">
         <v>43621</v>
@@ -1620,15 +1614,15 @@
     </row>
     <row r="34" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
       <c r="E34" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F34" s="14">
         <v>43621</v>
@@ -1637,15 +1631,15 @@
     </row>
     <row r="35" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
       <c r="E35" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F35" s="14">
         <v>43621</v>
@@ -1654,15 +1648,15 @@
     </row>
     <row r="36" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
       <c r="E36" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F36" s="14">
         <v>43621</v>
@@ -1671,15 +1665,15 @@
     </row>
     <row r="37" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
       <c r="E37" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F37" s="14">
         <v>43621</v>
@@ -1688,15 +1682,15 @@
     </row>
     <row r="38" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
       <c r="E38" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F38" s="14">
         <v>43621</v>
@@ -1705,15 +1699,15 @@
     </row>
     <row r="39" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
       <c r="E39" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F39" s="14">
         <v>43621</v>
@@ -1722,15 +1716,15 @@
     </row>
     <row r="40" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
       <c r="E40" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F40" s="14">
         <v>43621</v>
@@ -1739,37 +1733,23 @@
     </row>
     <row r="41" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
       <c r="E41" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F41" s="14">
         <v>43621</v>
       </c>
       <c r="G41" s="10"/>
     </row>
-    <row r="42" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="F42" s="14">
-        <v>43621</v>
-      </c>
-      <c r="G42" s="10"/>
+    <row r="42" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+      <c r="A42" s="15"/>
     </row>
     <row r="43" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A43" s="15"/>
@@ -1812,9 +1792,6 @@
     </row>
     <row r="56" spans="1:1" ht="18" x14ac:dyDescent="0.3">
       <c r="A56" s="15"/>
-    </row>
-    <row r="57" spans="1:1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A57" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
new questions have been added
</commit_message>
<xml_diff>
--- a/TAWA_SIQ.xlsx
+++ b/TAWA_SIQ.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="id">Sheet1!$I$642940</definedName>
+    <definedName name="id">Sheet1!$I$642939</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="116">
   <si>
     <t>From which source the top travel destinations appear statistics or ratings of the website?</t>
   </si>
@@ -338,9 +338,6 @@
     <t>what is the type of the  error message in the sign up and the login forms?</t>
   </si>
   <si>
-    <t>The submition of the signing up process  in the 'sign up' form is a link or a button ?</t>
-  </si>
-  <si>
     <t>Is there a 'login' link' in the sign up form?</t>
   </si>
   <si>
@@ -459,6 +456,52 @@
   </si>
   <si>
     <t>PENDING</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_040</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_041</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_042</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_043</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_044</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_045</t>
+  </si>
+  <si>
+    <t>TAWA_SIQ_046</t>
+  </si>
+  <si>
+    <t>The sign up button will be clickable all the time or after filling required fields only ?</t>
+  </si>
+  <si>
+    <t>What will happen if a user enters a "user name" which already exists ?</t>
+  </si>
+  <si>
+    <t>What are  the fields shall the admin fill to add a new user ?</t>
+  </si>
+  <si>
+    <t>How will the admin delete ?</t>
+  </si>
+  <si>
+    <t>Can admin delete more than one user at the same time ?</t>
+  </si>
+  <si>
+    <t>How will the payment methods option in booking form be displayed?</t>
+  </si>
+  <si>
+    <t>Submit button in booking form will be clickable all the time or after filling required fields only ?</t>
+  </si>
+  <si>
+    <t>Add button when the admin adds a new user
+will be clickable all the time or after filling required fields only ?</t>
   </si>
 </sst>
 </file>
@@ -633,7 +676,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -678,6 +721,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -985,10 +1031,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:A41"/>
+    <sheetView tabSelected="1" topLeftCell="D40" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1282,7 +1328,7 @@
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F14" s="14">
         <v>43621</v>
@@ -1299,7 +1345,7 @@
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
       <c r="E15" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F15" s="14">
         <v>43621</v>
@@ -1316,7 +1362,7 @@
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F16" s="14">
         <v>43621</v>
@@ -1333,7 +1379,7 @@
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F17" s="14">
         <v>43621</v>
@@ -1350,7 +1396,7 @@
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F18" s="14">
         <v>43621</v>
@@ -1362,12 +1408,12 @@
         <v>42</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F19" s="14">
         <v>43621</v>
@@ -1379,12 +1425,12 @@
         <v>43</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F20" s="14">
         <v>43621</v>
@@ -1396,12 +1442,12 @@
         <v>44</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
       <c r="E21" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F21" s="14">
         <v>43621</v>
@@ -1413,12 +1459,12 @@
         <v>45</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F22" s="14">
         <v>43621</v>
@@ -1430,12 +1476,12 @@
         <v>46</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
       <c r="E23" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F23" s="14">
         <v>43621</v>
@@ -1452,7 +1498,7 @@
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F24" s="14">
         <v>43621</v>
@@ -1461,7 +1507,7 @@
     </row>
     <row r="25" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>83</v>
@@ -1469,7 +1515,7 @@
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F25" s="14">
         <v>43621</v>
@@ -1478,7 +1524,7 @@
     </row>
     <row r="26" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>84</v>
@@ -1486,7 +1532,7 @@
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
       <c r="E26" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F26" s="14">
         <v>43621</v>
@@ -1495,7 +1541,7 @@
     </row>
     <row r="27" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>85</v>
@@ -1503,7 +1549,7 @@
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
       <c r="E27" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F27" s="14">
         <v>43621</v>
@@ -1512,15 +1558,15 @@
     </row>
     <row r="28" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
       <c r="E28" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F28" s="14">
         <v>43621</v>
@@ -1529,7 +1575,7 @@
     </row>
     <row r="29" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>88</v>
@@ -1537,7 +1583,7 @@
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
       <c r="E29" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F29" s="14">
         <v>43621</v>
@@ -1546,7 +1592,7 @@
     </row>
     <row r="30" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>89</v>
@@ -1554,7 +1600,7 @@
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
       <c r="E30" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F30" s="14">
         <v>43621</v>
@@ -1563,7 +1609,7 @@
     </row>
     <row r="31" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>90</v>
@@ -1571,7 +1617,7 @@
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
       <c r="E31" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F31" s="14">
         <v>43621</v>
@@ -1580,7 +1626,7 @@
     </row>
     <row r="32" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>91</v>
@@ -1588,7 +1634,7 @@
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
       <c r="E32" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F32" s="14">
         <v>43621</v>
@@ -1597,7 +1643,7 @@
     </row>
     <row r="33" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>92</v>
@@ -1605,7 +1651,7 @@
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
       <c r="E33" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F33" s="14">
         <v>43621</v>
@@ -1614,7 +1660,7 @@
     </row>
     <row r="34" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>93</v>
@@ -1622,7 +1668,7 @@
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
       <c r="E34" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F34" s="14">
         <v>43621</v>
@@ -1631,7 +1677,7 @@
     </row>
     <row r="35" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B35" s="11" t="s">
         <v>94</v>
@@ -1639,7 +1685,7 @@
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
       <c r="E35" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F35" s="14">
         <v>43621</v>
@@ -1648,7 +1694,7 @@
     </row>
     <row r="36" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>95</v>
@@ -1656,7 +1702,7 @@
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
       <c r="E36" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F36" s="14">
         <v>43621</v>
@@ -1665,7 +1711,7 @@
     </row>
     <row r="37" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>96</v>
@@ -1673,7 +1719,7 @@
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
       <c r="E37" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F37" s="14">
         <v>43621</v>
@@ -1682,7 +1728,7 @@
     </row>
     <row r="38" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B38" s="11" t="s">
         <v>97</v>
@@ -1690,7 +1736,7 @@
       <c r="C38" s="10"/>
       <c r="D38" s="10"/>
       <c r="E38" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F38" s="14">
         <v>43621</v>
@@ -1699,7 +1745,7 @@
     </row>
     <row r="39" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B39" s="11" t="s">
         <v>98</v>
@@ -1707,7 +1753,7 @@
       <c r="C39" s="10"/>
       <c r="D39" s="10"/>
       <c r="E39" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F39" s="14">
         <v>43621</v>
@@ -1716,7 +1762,7 @@
     </row>
     <row r="40" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B40" s="11" t="s">
         <v>99</v>
@@ -1724,50 +1770,148 @@
       <c r="C40" s="10"/>
       <c r="D40" s="10"/>
       <c r="E40" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F40" s="14">
         <v>43621</v>
       </c>
       <c r="G40" s="10"/>
     </row>
-    <row r="41" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>100</v>
+        <v>80</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
       <c r="E41" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="F41" s="14">
+        <v>43621</v>
+      </c>
+      <c r="G41" s="10"/>
+    </row>
+    <row r="42" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A42" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="F41" s="14">
-        <v>43621</v>
-      </c>
-      <c r="G41" s="10"/>
-    </row>
-    <row r="42" spans="1:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="A42" s="15"/>
-    </row>
-    <row r="43" spans="1:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="A43" s="15"/>
-    </row>
-    <row r="44" spans="1:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="A44" s="15"/>
-    </row>
-    <row r="45" spans="1:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="A45" s="15"/>
-    </row>
-    <row r="46" spans="1:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="A46" s="15"/>
-    </row>
-    <row r="47" spans="1:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="A47" s="15"/>
-    </row>
-    <row r="48" spans="1:7" ht="18" x14ac:dyDescent="0.3">
-      <c r="A48" s="15"/>
+      <c r="B42" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="F42" s="14">
+        <v>43621</v>
+      </c>
+      <c r="G42" s="10"/>
+    </row>
+    <row r="43" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A43" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="F43" s="14">
+        <v>43621</v>
+      </c>
+      <c r="G43" s="10"/>
+    </row>
+    <row r="44" spans="1:7" ht="36" x14ac:dyDescent="0.35">
+      <c r="A44" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="F44" s="14">
+        <v>43621</v>
+      </c>
+      <c r="G44" s="10"/>
+    </row>
+    <row r="45" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A45" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="F45" s="14">
+        <v>43621</v>
+      </c>
+      <c r="G45" s="10"/>
+    </row>
+    <row r="46" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A46" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="F46" s="14">
+        <v>43621</v>
+      </c>
+      <c r="G46" s="10"/>
+    </row>
+    <row r="47" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A47" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="F47" s="14">
+        <v>43621</v>
+      </c>
+      <c r="G47" s="10"/>
+    </row>
+    <row r="48" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A48" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="F48" s="14">
+        <v>43621</v>
+      </c>
+      <c r="G48" s="10"/>
     </row>
     <row r="49" spans="1:1" ht="18" x14ac:dyDescent="0.3">
       <c r="A49" s="15"/>
@@ -1789,9 +1933,6 @@
     </row>
     <row r="55" spans="1:1" ht="18" x14ac:dyDescent="0.3">
       <c r="A55" s="15"/>
-    </row>
-    <row r="56" spans="1:1" ht="18" x14ac:dyDescent="0.3">
-      <c r="A56" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>